<commit_message>
chumbak site automation completed
</commit_message>
<xml_diff>
--- a/test_input_data/CHUMBAK_DATA.xlsx
+++ b/test_input_data/CHUMBAK_DATA.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lnttsgroup-my.sharepoint.com/personal/aparna_mohanan_ltts_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Caption_Project\test_input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{822B457F-8E6A-4CA7-9E01-D1C0D242BDC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645C2066-999A-484A-A240-1BC60E8066F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0EAFDD02-D0E4-49AD-9972-D87A3418CDAD}"/>
   </bookViews>
   <sheets>
     <sheet name="Valid_Login_Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid_Login_Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>${firstname}</t>
   </si>
@@ -62,59 +63,107 @@
     <t>Valid_Login_4</t>
   </si>
   <si>
-    <t>aparnaml@gmail.com</t>
-  </si>
-  <si>
-    <t>doddy123</t>
-  </si>
-  <si>
-    <t>CA</t>
-  </si>
-  <si>
-    <t>SE</t>
-  </si>
-  <si>
-    <t>NI</t>
-  </si>
-  <si>
-    <t>AP</t>
-  </si>
-  <si>
-    <t>MO</t>
-  </si>
-  <si>
-    <t>KA</t>
-  </si>
-  <si>
-    <t>St</t>
-  </si>
-  <si>
-    <t>sccs</t>
-  </si>
-  <si>
-    <t>nika@gmail.com</t>
-  </si>
-  <si>
-    <t>loni@hotmail.com</t>
-  </si>
-  <si>
-    <t>poi@dmail.com</t>
-  </si>
-  <si>
-    <t>nmbnvjg789</t>
-  </si>
-  <si>
-    <t>hbhjgy687</t>
-  </si>
-  <si>
-    <t>bhghg7080</t>
+    <t>APARNA</t>
+  </si>
+  <si>
+    <t>MOHANAN</t>
+  </si>
+  <si>
+    <t>NIKHIL</t>
+  </si>
+  <si>
+    <t>KANAN</t>
+  </si>
+  <si>
+    <t>SELSHIYA</t>
+  </si>
+  <si>
+    <t>STEPHEN</t>
+  </si>
+  <si>
+    <t>CALLY</t>
+  </si>
+  <si>
+    <t>JOSEPH</t>
+  </si>
+  <si>
+    <t>aparnamohanan@gmail.com</t>
+  </si>
+  <si>
+    <t>nikilkanan@gmail.com</t>
+  </si>
+  <si>
+    <t>selstephen@hotmail.com</t>
+  </si>
+  <si>
+    <t>caljoe@dmail.com</t>
+  </si>
+  <si>
+    <t>Joe_cal23</t>
+  </si>
+  <si>
+    <t>selshiya677</t>
+  </si>
+  <si>
+    <t>kanan_90nik</t>
+  </si>
+  <si>
+    <t>aparna_123</t>
+  </si>
+  <si>
+    <t>${expected_msg}</t>
+  </si>
+  <si>
+    <t>reset your password</t>
+  </si>
+  <si>
+    <t>Invalid_Login_1</t>
+  </si>
+  <si>
+    <t>Invalid_Login_2</t>
+  </si>
+  <si>
+    <t>Invalid_Login_3</t>
+  </si>
+  <si>
+    <t>Invalid_Login_4</t>
+  </si>
+  <si>
+    <t>siva12345</t>
+  </si>
+  <si>
+    <t>ras_890moh</t>
+  </si>
+  <si>
+    <t>surya_456</t>
+  </si>
+  <si>
+    <t>thangam34</t>
+  </si>
+  <si>
+    <t>${expected_error}</t>
+  </si>
+  <si>
+    <t>Incorrect email or password.</t>
+  </si>
+  <si>
+    <t>sivabalan@gmail.com</t>
+  </si>
+  <si>
+    <t>rasmoh@gmail.com</t>
+  </si>
+  <si>
+    <t>nirmal@hotmail.com</t>
+  </si>
+  <si>
+    <t>lekshmi@hotmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +175,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -152,9 +207,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -470,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D12238D3-1849-4B1E-B2A0-51D77111E69F}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,11 +539,13 @@
     <col min="1" max="1" width="13.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.109375" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="21.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" customWidth="1"/>
     <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="49.33203125" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -501,73 +561,88 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>22</v>
+      </c>
+      <c r="F4" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
-        <v>24</v>
+      <c r="F5" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -576,6 +651,107 @@
     <hyperlink ref="D3" r:id="rId2" xr:uid="{6AC27EB4-F3F6-46DF-A2A5-A093249C26F8}"/>
     <hyperlink ref="D4" r:id="rId3" xr:uid="{4506CC77-0790-4D6A-B33E-4C68EC7A4859}"/>
     <hyperlink ref="D5" r:id="rId4" xr:uid="{BB77D4B4-902B-4AC7-A4E9-87EA9EA36061}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0EB58E-E1C6-4E5E-B418-5DCC0495AC6A}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{17F2D8F3-64DB-4318-815F-5D91EE5918D0}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{6D7C12EC-286B-40A9-9FF4-6B1B9746A89E}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{E591DCA5-5E44-437F-A0C4-186A8D0454E4}"/>
+    <hyperlink ref="B5" r:id="rId4" xr:uid="{B17704DD-E2E5-4CDE-A766-0B4DA1C1962C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
CHUMBAK WEBSITE ----> COMPLETED
</commit_message>
<xml_diff>
--- a/test_input_data/CHUMBAK_DATA.xlsx
+++ b/test_input_data/CHUMBAK_DATA.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Caption_Project\test_input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645C2066-999A-484A-A240-1BC60E8066F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10796E60-7AC6-400B-B25A-EE2C572E833E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0EAFDD02-D0E4-49AD-9972-D87A3418CDAD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Valid_Login_Test" sheetId="1" r:id="rId1"/>
-    <sheet name="Invalid_Login_Test" sheetId="2" r:id="rId2"/>
+    <sheet name="Valid_Register_Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Invalid_Register_Test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>${firstname}</t>
   </si>
@@ -129,24 +129,9 @@
     <t>Invalid_Login_4</t>
   </si>
   <si>
-    <t>siva12345</t>
-  </si>
-  <si>
-    <t>ras_890moh</t>
-  </si>
-  <si>
-    <t>surya_456</t>
-  </si>
-  <si>
-    <t>thangam34</t>
-  </si>
-  <si>
     <t>${expected_error}</t>
   </si>
   <si>
-    <t>Incorrect email or password.</t>
-  </si>
-  <si>
     <t>sivabalan@gmail.com</t>
   </si>
   <si>
@@ -157,6 +142,45 @@
   </si>
   <si>
     <t>lekshmi@hotmail.com</t>
+  </si>
+  <si>
+    <t>siva</t>
+  </si>
+  <si>
+    <t>balan</t>
+  </si>
+  <si>
+    <t>rashmika</t>
+  </si>
+  <si>
+    <t>mohammed</t>
+  </si>
+  <si>
+    <t>nirmala</t>
+  </si>
+  <si>
+    <t>raikumar</t>
+  </si>
+  <si>
+    <t>lekshmi</t>
+  </si>
+  <si>
+    <t>thangam</t>
+  </si>
+  <si>
+    <t>tan</t>
+  </si>
+  <si>
+    <t>wer1</t>
+  </si>
+  <si>
+    <t>ai_8</t>
+  </si>
+  <si>
+    <t>rt@w</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is too short (minimum is 5 characters)</t>
   </si>
 </sst>
 </file>
@@ -531,7 +555,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C1" sqref="C1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,7 +686,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,7 +696,7 @@
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="25.33203125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="36.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -680,81 +704,111 @@
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>35</v>
+      <c r="F1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="2"/>
+      <c r="D2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
         <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
+        <v>39</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>39</v>
+      <c r="B4" t="s">
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" t="s">
-        <v>36</v>
+        <v>41</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>40</v>
+      <c r="B5" t="s">
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
+        <v>43</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{17F2D8F3-64DB-4318-815F-5D91EE5918D0}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{6D7C12EC-286B-40A9-9FF4-6B1B9746A89E}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{E591DCA5-5E44-437F-A0C4-186A8D0454E4}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{B17704DD-E2E5-4CDE-A766-0B4DA1C1962C}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{31AA5520-EBBA-494E-8DF0-C30609E66B2A}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{989D4595-374F-4DEE-8851-8CD11376C650}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{F9378EC2-981C-47C9-8F39-5F0B2FB83A68}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{E94F0658-E95A-4826-A9F4-55127C9CA2C2}"/>
+    <hyperlink ref="E3" r:id="rId5" xr:uid="{B48D1A22-7C36-4D8B-B777-40A6B624EDEA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
@@ -956,18 +1010,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -990,18 +1044,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E23DC92B-DD78-47ED-BE36-E8C3A7E054DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A93E885A-C220-46DE-B05B-09FD51142317}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E23DC92B-DD78-47ED-BE36-E8C3A7E054DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>